<commit_message>
import product from excel
</commit_message>
<xml_diff>
--- a/static/products.xlsx
+++ b/static/products.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,10 +44,10 @@
     <t>steel rod</t>
   </si>
   <si>
-    <t>quality 3</t>
-  </si>
-  <si>
-    <t>quality 2</t>
+    <t>good quality</t>
+  </si>
+  <si>
+    <t>perfect condition</t>
   </si>
 </sst>
 </file>
@@ -368,10 +368,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -391,7 +396,13 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -399,7 +410,13 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>